<commit_message>
Changed lcsc part number for 33nF cap
</commit_message>
<xml_diff>
--- a/Hardware/Cornverter LCSC BOM.xlsx
+++ b/Hardware/Cornverter LCSC BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Cornverter\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D785A255-134B-4FE1-8686-7E152F7828F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E329EBBD-81A9-4C0C-9AB0-FA83191BCD1E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{33667046-9C3D-47AC-83F4-8537F7000775}"/>
   </bookViews>
@@ -273,9 +273,6 @@
     <t>33nF Ceramic Capacitor</t>
   </si>
   <si>
-    <t>C1906</t>
-  </si>
-  <si>
     <t>Amount Spare</t>
   </si>
   <si>
@@ -391,6 +388,9 @@
   </si>
   <si>
     <t>Ebay Shipping</t>
+  </si>
+  <si>
+    <t>C97930</t>
   </si>
 </sst>
 </file>
@@ -818,11 +818,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F513871-9508-4665-AE19-3C0D704DA94E}">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,7 +850,7 @@
         <v>64</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>65</v>
@@ -1115,7 +1115,7 @@
       <c r="H10" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="4" t="s">
         <v>70</v>
       </c>
       <c r="J10" s="4" t="s">
@@ -1154,7 +1154,7 @@
         <v>3.0300000000000001E-3</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" ref="G11:G50" si="2">D11*F11</f>
+        <f>D11*F11</f>
         <v>0.2424</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -1198,7 +1198,7 @@
         <v>7.8700000000000006E-2</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G11:G50" si="2">D12*F12</f>
         <v>0.39350000000000002</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -1281,7 +1281,7 @@
         <v>69</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>3</v>
@@ -1419,27 +1419,27 @@
         <v>4</v>
       </c>
       <c r="C18" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D18" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F18" s="2">
-        <v>2.9499999999999998E-2</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" si="2"/>
-        <v>0.29499999999999998</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>78</v>
@@ -1480,7 +1480,7 @@
         <v>69</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>18</v>
@@ -1518,7 +1518,7 @@
         <v>69</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>59</v>
@@ -1553,10 +1553,10 @@
         <v>3.7199999999999998</v>
       </c>
       <c r="H21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>8</v>
@@ -1594,7 +1594,7 @@
         <v>69</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>60</v>
@@ -1632,7 +1632,7 @@
         <v>69</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>17</v>
@@ -1670,7 +1670,7 @@
         <v>69</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>19</v>
@@ -1679,7 +1679,7 @@
         <v>20</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1711,13 +1711,13 @@
         <v>69</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1749,7 +1749,7 @@
         <v>69</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>22</v>
@@ -1787,7 +1787,7 @@
         <v>69</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>24</v>
@@ -1825,7 +1825,7 @@
         <v>69</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>25</v>
@@ -1866,7 +1866,7 @@
         <v>69</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>26</v>
@@ -1907,7 +1907,7 @@
         <v>69</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>27</v>
@@ -1948,7 +1948,7 @@
         <v>69</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>28</v>
@@ -1989,7 +1989,7 @@
         <v>69</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>29</v>
@@ -2030,7 +2030,7 @@
         <v>69</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>30</v>
@@ -2071,7 +2071,7 @@
         <v>69</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>31</v>
@@ -2112,7 +2112,7 @@
         <v>69</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>32</v>
@@ -2153,7 +2153,7 @@
         <v>69</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>33</v>
@@ -2194,13 +2194,13 @@
         <v>69</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2232,13 +2232,13 @@
         <v>69</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2270,7 +2270,7 @@
         <v>69</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>36</v>
@@ -2308,13 +2308,13 @@
         <v>69</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>38</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2346,7 +2346,7 @@
         <v>69</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>39</v>
@@ -2382,7 +2382,7 @@
         <v>16.322222222222223</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>42</v>
@@ -2421,7 +2421,7 @@
         <v>2.8249999999999997</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>43</v>
@@ -2457,10 +2457,10 @@
         <v>1.8000000000000003</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2487,10 +2487,10 @@
         <v>1.8000000000000003</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2530,10 +2530,10 @@
         <v>1.54</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -2558,7 +2558,7 @@
         <v>69</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2580,10 +2580,10 @@
         <v>2.95</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -2605,10 +2605,10 @@
         <v>0</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -2622,18 +2622,24 @@
       </c>
       <c r="D52" s="2">
         <f>SUM(D10:D50)</f>
-        <v>1078</v>
+        <v>1073</v>
       </c>
       <c r="E52" s="2">
         <f>SUM(E10:E50)</f>
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="G52" s="2">
         <f>SUM(G10:G50)</f>
-        <v>52.409522222222215</v>
+        <v>52.589522222222215</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G56" s="2">
+        <f>SUM(G10:G41)-G21</f>
+        <v>16.012299999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected price of cd4050 in bom
</commit_message>
<xml_diff>
--- a/Hardware/Cornverter LCSC BOM.xlsx
+++ b/Hardware/Cornverter LCSC BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Cornverter\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E329EBBD-81A9-4C0C-9AB0-FA83191BCD1E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0F3258-37A2-4DA7-A9AC-37DD4DC414FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{33667046-9C3D-47AC-83F4-8537F7000775}"/>
   </bookViews>
@@ -821,8 +821,8 @@
   <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2222,11 +2222,11 @@
         <v>2</v>
       </c>
       <c r="F38" s="2">
-        <v>0.16370000000000001</v>
+        <v>0.1225</v>
       </c>
       <c r="G38" s="2">
         <f t="shared" si="2"/>
-        <v>1.637</v>
+        <v>1.2250000000000001</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>69</v>
@@ -2630,7 +2630,7 @@
       </c>
       <c r="G52" s="2">
         <f>SUM(G10:G50)</f>
-        <v>52.589522222222215</v>
+        <v>52.177522222222208</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>62</v>
@@ -2639,7 +2639,7 @@
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G56" s="2">
         <f>SUM(G10:G41)-G21</f>
-        <v>16.012299999999996</v>
+        <v>15.600299999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ebay burchase to excel
</commit_message>
<xml_diff>
--- a/Hardware/Cornverter LCSC BOM.xlsx
+++ b/Hardware/Cornverter LCSC BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Cornverter\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0F3258-37A2-4DA7-A9AC-37DD4DC414FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D271381C-1966-4ABC-A42F-749BB410159A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{33667046-9C3D-47AC-83F4-8537F7000775}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="122">
   <si>
     <t>Quantity</t>
   </si>
@@ -391,12 +391,24 @@
   </si>
   <si>
     <t>C97930</t>
+  </si>
+  <si>
+    <t>Purchased?</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Amount Spent:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,7 +470,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -481,13 +493,50 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{CA88BD54-F734-41BA-967D-5A9BFDB6E4F4}"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -818,11 +867,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F513871-9508-4665-AE19-3C0D704DA94E}">
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +885,7 @@
     <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -876,8 +925,11 @@
       <c r="M1" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>3</v>
       </c>
@@ -903,7 +955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -929,7 +981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>4</v>
       </c>
@@ -955,7 +1007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -981,7 +1033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>1</v>
       </c>
@@ -1007,7 +1059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -1033,7 +1085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>2</v>
       </c>
@@ -1059,7 +1111,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>2</v>
       </c>
@@ -1085,7 +1137,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>M10</f>
         <v>39</v>
@@ -1130,7 +1182,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>M11</f>
         <v>37</v>
@@ -1175,7 +1227,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2</v>
       </c>
@@ -1214,7 +1266,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1</v>
       </c>
@@ -1252,7 +1304,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>2</v>
       </c>
@@ -1287,7 +1339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1328,7 +1380,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>8</v>
       </c>
@@ -2374,12 +2426,12 @@
         <v>4</v>
       </c>
       <c r="F42" s="2">
-        <f>14.69/36</f>
-        <v>0.40805555555555556</v>
+        <f>16.32/40</f>
+        <v>0.40800000000000003</v>
       </c>
       <c r="G42" s="2">
         <f t="shared" si="2"/>
-        <v>16.322222222222223</v>
+        <v>16.32</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>109</v>
@@ -2413,12 +2465,12 @@
         <v>3</v>
       </c>
       <c r="F43" s="2">
-        <f>1.13/2</f>
-        <v>0.56499999999999995</v>
+        <f>2.82/5</f>
+        <v>0.56399999999999995</v>
       </c>
       <c r="G43" s="2">
         <f t="shared" si="2"/>
-        <v>2.8249999999999997</v>
+        <v>2.82</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>109</v>
@@ -2573,11 +2625,11 @@
         <v>0</v>
       </c>
       <c r="F49" s="2">
-        <v>2.95</v>
+        <v>0</v>
       </c>
       <c r="G49" s="2">
         <f t="shared" si="2"/>
-        <v>2.95</v>
+        <v>0</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>109</v>
@@ -2630,22 +2682,37 @@
       </c>
       <c r="G52" s="2">
         <f>SUM(G10:G50)</f>
-        <v>52.177522222222208</v>
+        <v>49.220299999999988</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G56" s="2">
-        <f>SUM(G10:G41)-G21</f>
-        <v>15.600299999999994</v>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C54" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C55" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D55" s="8">
+        <v>3.72</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E10:E50">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N45">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"y"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Forgot to save before previous commit
</commit_message>
<xml_diff>
--- a/Hardware/Cornverter LCSC BOM.xlsx
+++ b/Hardware/Cornverter LCSC BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Cornverter\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D271381C-1966-4ABC-A42F-749BB410159A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEA8780-C855-4A3E-8FF6-684FB44168C5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{33667046-9C3D-47AC-83F4-8537F7000775}"/>
   </bookViews>
@@ -869,9 +869,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F513871-9508-4665-AE19-3C0D704DA94E}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
forgot to save before previous commit again whoops
</commit_message>
<xml_diff>
--- a/Hardware/Cornverter LCSC BOM.xlsx
+++ b/Hardware/Cornverter LCSC BOM.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Cornverter\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEA8780-C855-4A3E-8FF6-684FB44168C5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C74F73-EBBB-4F7D-A07E-5D387D551AC2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{33667046-9C3D-47AC-83F4-8537F7000775}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="123">
   <si>
     <t>Quantity</t>
   </si>
@@ -400,6 +397,9 @@
   </si>
   <si>
     <t>Amount Spent:</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -502,7 +502,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{CA88BD54-F734-41BA-967D-5A9BFDB6E4F4}"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -510,30 +510,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -555,19 +531,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cornverter BOM 2019 02 09"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -869,15 +832,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F513871-9508-4665-AE19-3C0D704DA94E}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54:B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="8.7109375" style="2" customWidth="1"/>
+    <col min="2" max="7" width="8.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="18.140625" style="2" customWidth="1"/>
     <col min="10" max="10" width="24.140625" style="2" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -1250,7 +1214,7 @@
         <v>7.8700000000000006E-2</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" ref="G11:G50" si="2">D12*F12</f>
+        <f t="shared" ref="G12:G50" si="2">D12*F12</f>
         <v>0.39350000000000002</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -1421,7 +1385,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>2</v>
       </c>
@@ -1462,7 +1426,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>2</v>
       </c>
@@ -1503,7 +1467,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>1</v>
       </c>
@@ -1541,7 +1505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -1579,7 +1543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>1</v>
       </c>
@@ -1616,8 +1580,11 @@
       <c r="K21" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N21" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1</v>
       </c>
@@ -1655,7 +1622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>3</v>
       </c>
@@ -1693,7 +1660,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>3</v>
       </c>
@@ -1734,7 +1701,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>1</v>
       </c>
@@ -1772,7 +1739,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>12</v>
       </c>
@@ -1810,7 +1777,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>6</v>
       </c>
@@ -1848,7 +1815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>1</v>
       </c>
@@ -1889,7 +1856,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>1</v>
       </c>
@@ -1930,7 +1897,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>16</v>
       </c>
@@ -1971,7 +1938,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>2</v>
       </c>
@@ -2012,7 +1979,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>2</v>
       </c>
@@ -2689,29 +2656,29 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C54" s="2" t="s">
+      <c r="A54" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C55" s="2" t="s">
+      <c r="A55" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D55" s="8">
+      <c r="B55" s="8">
         <v>3.72</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E10:E50">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N45">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added jumpers to BOM
</commit_message>
<xml_diff>
--- a/Hardware/Cornverter LCSC BOM.xlsx
+++ b/Hardware/Cornverter LCSC BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Cornverter\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C74F73-EBBB-4F7D-A07E-5D387D551AC2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A59309B-DF30-4920-9591-E1305E9A68D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{33667046-9C3D-47AC-83F4-8537F7000775}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="125">
   <si>
     <t>Quantity</t>
   </si>
@@ -400,6 +400,12 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>1x2 Female Jumper</t>
+  </si>
+  <si>
+    <t>C100114</t>
   </si>
 </sst>
 </file>
@@ -830,11 +836,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F513871-9508-4665-AE19-3C0D704DA94E}">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:N56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54:B55"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +930,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5">
-        <f t="shared" ref="B3:B47" si="0">A3*2</f>
+        <f t="shared" ref="B3:B48" si="0">A3*2</f>
         <v>4</v>
       </c>
       <c r="C3" s="5"/>
@@ -1162,7 +1168,7 @@
         <v>80</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" ref="E11:E50" si="1">IF(D11&gt;0, D11-B11, "")</f>
+        <f t="shared" ref="E11:E51" si="1">IF(D11&gt;0, D11-B11, "")</f>
         <v>6</v>
       </c>
       <c r="F11" s="2">
@@ -1214,7 +1220,7 @@
         <v>7.8700000000000006E-2</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" ref="G12:G50" si="2">D12*F12</f>
+        <f t="shared" ref="G12:G51" si="2">D12*F12</f>
         <v>0.39350000000000002</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -1270,113 +1276,110 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C14" s="2">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="D14" s="2">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="F14" s="2">
-        <v>8.5099999999999995E-2</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="2"/>
-        <v>0.42549999999999999</v>
+        <v>0.21</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>3</v>
+        <v>123</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C15" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D15" s="2">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F15" s="2">
-        <v>3.0200000000000001E-2</v>
+        <v>8.5099999999999995E-2</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="2"/>
-        <v>0.90600000000000003</v>
+        <v>0.42549999999999999</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K15" s="2">
-        <v>1206</v>
-      </c>
-      <c r="L15" s="7">
-        <v>0.05</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C16" s="2">
         <v>10</v>
       </c>
       <c r="D16" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="F16" s="2">
-        <v>2.87E-2</v>
+        <v>3.0200000000000001E-2</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="2"/>
-        <v>0.57399999999999995</v>
+        <v>0.90600000000000003</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K16" s="2">
         <v>1206</v>
@@ -1387,37 +1390,37 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D17" s="2">
         <v>20</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F17" s="2">
-        <v>2.0899999999999998E-2</v>
+        <v>2.87E-2</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" si="2"/>
-        <v>0.41799999999999998</v>
+        <v>0.57399999999999995</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K17" s="2">
         <v>1206</v>
@@ -1435,30 +1438,30 @@
         <v>4</v>
       </c>
       <c r="C18" s="2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D18" s="2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F18" s="2">
-        <v>9.5000000000000001E-2</v>
+        <v>2.0899999999999998E-2</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" si="2"/>
-        <v>0.47499999999999998</v>
+        <v>0.41799999999999998</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="K18" s="2">
         <v>1206</v>
@@ -1469,40 +1472,43 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C19" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D19" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="2">
-        <v>0.43859999999999999</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="2"/>
-        <v>0.87719999999999998</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>7</v>
+        <v>78</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1206</v>
+      </c>
+      <c r="L19" s="7">
+        <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1517,27 +1523,27 @@
         <v>1</v>
       </c>
       <c r="D20" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F20" s="2">
-        <v>0.125</v>
+        <v>0.43859999999999999</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="2"/>
-        <v>0.625</v>
+        <v>0.87719999999999998</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>7</v>
@@ -1555,33 +1561,30 @@
         <v>1</v>
       </c>
       <c r="D21" s="2">
+        <v>5</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E21" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="F21" s="2">
-        <v>1.24</v>
+        <v>0.125</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="2"/>
-        <v>3.7199999999999998</v>
+        <v>0.625</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>115</v>
+        <v>69</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1593,71 +1596,74 @@
         <v>2</v>
       </c>
       <c r="C22" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F22" s="2">
-        <v>5.11E-2</v>
+        <v>1.24</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="2"/>
-        <v>0.2555</v>
+        <v>3.7199999999999998</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="N22" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2">
+        <v>5</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B23" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C23" s="2">
-        <v>50</v>
-      </c>
-      <c r="D23" s="2">
-        <v>50</v>
-      </c>
-      <c r="E23" s="2">
-        <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
       <c r="F23" s="2">
-        <v>4.4999999999999997E-3</v>
+        <v>5.11E-2</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="2"/>
-        <v>0.22499999999999998</v>
+        <v>0.2555</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1679,137 +1685,137 @@
         <v>44</v>
       </c>
       <c r="F24" s="2">
-        <v>6.7999999999999996E-3</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" si="2"/>
-        <v>0.33999999999999997</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L24" s="7" t="s">
-        <v>84</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B25" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C25" s="2">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="D25" s="2">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="F25" s="2">
-        <v>6.0699999999999997E-2</v>
+        <v>6.7999999999999996E-3</v>
       </c>
       <c r="G25" s="2">
         <f t="shared" si="2"/>
-        <v>0.30349999999999999</v>
+        <v>0.33999999999999997</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>86</v>
+        <v>20</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B26" s="2">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C26" s="2">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D26" s="2">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F26" s="2">
-        <v>1.6199999999999999E-2</v>
+        <v>6.0699999999999997E-2</v>
       </c>
       <c r="G26" s="2">
         <f t="shared" si="2"/>
-        <v>0.64799999999999991</v>
+        <v>0.30349999999999999</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B27" s="2">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C27" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D27" s="2">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F27" s="2">
-        <v>0.05</v>
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="G27" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.64799999999999991</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>23</v>
@@ -1817,43 +1823,40 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B28" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C28" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D28" s="2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="F28" s="2">
-        <v>3.0999999999999999E-3</v>
+        <v>0.05</v>
       </c>
       <c r="G28" s="2">
         <f t="shared" si="2"/>
-        <v>0.155</v>
+        <v>1</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K28" s="2">
-        <v>1206</v>
-      </c>
-      <c r="L28" s="7">
-        <v>0.01</v>
+        <v>24</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -1875,20 +1878,20 @@
         <v>48</v>
       </c>
       <c r="F29" s="2">
-        <v>2.8E-3</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="G29" s="2">
         <f t="shared" si="2"/>
-        <v>0.13999999999999999</v>
+        <v>0.155</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K29" s="2">
         <v>1206</v>
@@ -1899,11 +1902,11 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B30" s="2">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="C30" s="2">
         <v>50</v>
@@ -1913,23 +1916,23 @@
       </c>
       <c r="E30" s="2">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="F30" s="2">
-        <v>3.3E-3</v>
+        <v>2.8E-3</v>
       </c>
       <c r="G30" s="2">
         <f t="shared" si="2"/>
-        <v>0.16500000000000001</v>
+        <v>0.13999999999999999</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K30" s="2">
         <v>1206</v>
@@ -1940,11 +1943,11 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B31" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C31" s="2">
         <v>50</v>
@@ -1954,23 +1957,23 @@
       </c>
       <c r="E31" s="2">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F31" s="2">
-        <v>2.8E-3</v>
+        <v>3.3E-3</v>
       </c>
       <c r="G31" s="2">
         <f t="shared" si="2"/>
-        <v>0.13999999999999999</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K31" s="2">
         <v>1206</v>
@@ -1998,20 +2001,20 @@
         <v>46</v>
       </c>
       <c r="F32" s="2">
-        <v>4.4999999999999997E-3</v>
+        <v>2.8E-3</v>
       </c>
       <c r="G32" s="2">
         <f t="shared" si="2"/>
-        <v>0.22499999999999998</v>
+        <v>0.13999999999999999</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K32" s="2">
         <v>1206</v>
@@ -2022,11 +2025,11 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C33" s="2">
         <v>50</v>
@@ -2036,23 +2039,23 @@
       </c>
       <c r="E33" s="2">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F33" s="2">
-        <v>2.8999999999999998E-3</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="G33" s="2">
         <f t="shared" si="2"/>
-        <v>0.14499999999999999</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K33" s="2">
         <v>1206</v>
@@ -2063,11 +2066,11 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B34" s="2">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="C34" s="2">
         <v>50</v>
@@ -2077,23 +2080,23 @@
       </c>
       <c r="E34" s="2">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="F34" s="2">
-        <v>3.0999999999999999E-3</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="G34" s="2">
         <f t="shared" si="2"/>
-        <v>0.155</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K34" s="2">
         <v>1206</v>
@@ -2104,37 +2107,37 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B35" s="2">
         <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="C35" s="2">
+        <v>50</v>
+      </c>
+      <c r="D35" s="2">
+        <v>50</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C35" s="2">
-        <v>50</v>
-      </c>
-      <c r="D35" s="2">
-        <v>50</v>
-      </c>
-      <c r="E35" s="2">
-        <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
       <c r="F35" s="2">
-        <v>2.7000000000000001E-3</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="G35" s="2">
         <f t="shared" si="2"/>
-        <v>0.13500000000000001</v>
+        <v>0.155</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K35" s="2">
         <v>1206</v>
@@ -2145,11 +2148,11 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B36" s="2">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C36" s="2">
         <v>50</v>
@@ -2159,23 +2162,23 @@
       </c>
       <c r="E36" s="2">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F36" s="2">
-        <v>3.0000000000000001E-3</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="G36" s="2">
         <f t="shared" si="2"/>
-        <v>0.15</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K36" s="2">
         <v>1206</v>
@@ -2186,154 +2189,157 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B37" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C37" s="2">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D37" s="2">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="F37" s="2">
-        <v>0.1525</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="G37" s="2">
         <f t="shared" si="2"/>
-        <v>0.76249999999999996</v>
+        <v>0.15</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>102</v>
+        <v>33</v>
+      </c>
+      <c r="K37" s="2">
+        <v>1206</v>
+      </c>
+      <c r="L37" s="7">
+        <v>0.01</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
+        <v>2</v>
+      </c>
+      <c r="B38" s="2">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B38" s="2">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
       <c r="C38" s="2">
         <v>1</v>
       </c>
       <c r="D38" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E38" s="2">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" s="2">
-        <v>0.1225</v>
+        <v>0.1525</v>
       </c>
       <c r="G38" s="2">
         <f t="shared" si="2"/>
-        <v>1.2250000000000001</v>
+        <v>0.76249999999999996</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B39" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C39" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D39" s="2">
         <v>10</v>
       </c>
       <c r="E39" s="2">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F39" s="2">
-        <v>2.6599999999999999E-2</v>
+        <v>0.1225</v>
       </c>
       <c r="G39" s="2">
         <f t="shared" si="2"/>
-        <v>0.26600000000000001</v>
+        <v>1.2250000000000001</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>37</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B40" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C40" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D40" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E40" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F40" s="2">
-        <v>1.6158999999999999</v>
+        <v>2.6599999999999999E-2</v>
       </c>
       <c r="G40" s="2">
         <f t="shared" si="2"/>
-        <v>3.2317999999999998</v>
+        <v>0.26600000000000001</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>100</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2348,143 +2354,151 @@
         <v>1</v>
       </c>
       <c r="D41" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E41" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" s="2">
-        <v>0.14380000000000001</v>
+        <v>1.6158999999999999</v>
       </c>
       <c r="G41" s="2">
         <f t="shared" si="2"/>
-        <v>0.43140000000000001</v>
+        <v>3.2317999999999998</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>69</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
+        <v>1</v>
+      </c>
+      <c r="B42" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C42" s="2">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2">
+        <v>3</v>
+      </c>
+      <c r="E42" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.14380000000000001</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="2"/>
+        <v>0.43140000000000001</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
         <v>18</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B43" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="C42" s="2">
-        <v>1</v>
-      </c>
-      <c r="D42" s="2">
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2">
         <v>40</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E43" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F43" s="2">
         <f>16.32/40</f>
         <v>0.40800000000000003</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G43" s="2">
         <f t="shared" si="2"/>
         <v>16.32</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I42" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="J43" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K42" s="2" t="s">
+      <c r="K43" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <v>1</v>
-      </c>
-      <c r="B43" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C43" s="2">
-        <v>1</v>
-      </c>
-      <c r="D43" s="2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>1</v>
+      </c>
+      <c r="B44" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2">
         <v>5</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E44" s="2">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F44" s="2">
         <f>2.82/5</f>
         <v>0.56399999999999995</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G44" s="2">
         <f t="shared" si="2"/>
         <v>2.82</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="2">
-        <f>D42+D43</f>
-        <v>45</v>
-      </c>
-      <c r="C44" s="2">
-        <v>50</v>
-      </c>
-      <c r="D44" s="2">
-        <v>50</v>
-      </c>
-      <c r="E44" s="2">
-        <f>IF(D44&gt;0, D44-B44, "")</f>
-        <v>5</v>
-      </c>
-      <c r="F44" s="2">
-        <f>1.8/50</f>
-        <v>3.6000000000000004E-2</v>
-      </c>
-      <c r="G44" s="2">
-        <f t="shared" si="2"/>
-        <v>1.8000000000000003</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>109</v>
       </c>
+      <c r="I44" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="J44" s="2" t="s">
-        <v>107</v>
+        <v>44</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
-        <f>B44</f>
+        <f>D43+D44</f>
         <v>45</v>
       </c>
       <c r="C45" s="2">
@@ -2509,75 +2523,80 @@
         <v>109</v>
       </c>
       <c r="J45" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="2">
+        <f>B45</f>
+        <v>45</v>
+      </c>
+      <c r="C46" s="2">
+        <v>50</v>
+      </c>
+      <c r="D46" s="2">
+        <v>50</v>
+      </c>
+      <c r="E46" s="2">
+        <f>IF(D46&gt;0, D46-B46, "")</f>
+        <v>5</v>
+      </c>
+      <c r="F46" s="2">
+        <f>1.8/50</f>
+        <v>3.6000000000000004E-2</v>
+      </c>
+      <c r="G46" s="2">
+        <f t="shared" si="2"/>
+        <v>1.8000000000000003</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J46" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E46" s="2" t="str">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E47" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G46" s="2">
+      <c r="G47" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
-        <v>1</v>
-      </c>
-      <c r="B47" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C47" s="2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>1</v>
+      </c>
+      <c r="B48" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C48" s="2">
         <v>10</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D48" s="2">
         <v>10</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E48" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F48" s="2">
         <f>1.54/10</f>
         <v>0.154</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G48" s="2">
         <f t="shared" si="2"/>
         <v>1.54</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="H48" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="J47" s="2" t="s">
+      <c r="J48" s="2" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B48" s="2">
-        <v>1</v>
-      </c>
-      <c r="D48" s="2">
-        <v>1</v>
-      </c>
-      <c r="E48" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F48" s="2">
-        <v>5.62</v>
-      </c>
-      <c r="G48" s="2">
-        <f t="shared" si="2"/>
-        <v>5.62</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2592,17 +2611,17 @@
         <v>0</v>
       </c>
       <c r="F49" s="2">
-        <v>0</v>
+        <v>5.62</v>
       </c>
       <c r="G49" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.62</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -2624,64 +2643,90 @@
         <v>0</v>
       </c>
       <c r="H50" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="2">
+        <v>1</v>
+      </c>
+      <c r="D51" s="2">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0</v>
+      </c>
+      <c r="G51" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H51" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="J50" s="2" t="s">
+      <c r="J51" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
-        <f>SUM(A10:A49)</f>
-        <v>221</v>
-      </c>
-      <c r="B52" s="2">
-        <f>SUM(B10:B49)</f>
-        <v>534</v>
-      </c>
-      <c r="D52" s="2">
-        <f>SUM(D10:D50)</f>
-        <v>1073</v>
-      </c>
-      <c r="E52" s="2">
-        <f>SUM(E10:E50)</f>
-        <v>538</v>
-      </c>
-      <c r="G52" s="2">
-        <f>SUM(G10:G50)</f>
-        <v>49.220299999999988</v>
-      </c>
-      <c r="J52" s="2" t="s">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <f>SUM(A10:A50)</f>
+        <v>224</v>
+      </c>
+      <c r="B53" s="2">
+        <f>SUM(B10:B50)</f>
+        <v>540</v>
+      </c>
+      <c r="D53" s="2">
+        <f>SUM(D10:D51)</f>
+        <v>1123</v>
+      </c>
+      <c r="E53" s="2">
+        <f>SUM(E10:E51)</f>
+        <v>582</v>
+      </c>
+      <c r="G53" s="2">
+        <f>SUM(G10:G51)</f>
+        <v>49.430299999999981</v>
+      </c>
+      <c r="J53" s="2" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B55" s="8">
+      <c r="B56" s="8">
         <v>3.72</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E10:E50">
+  <conditionalFormatting sqref="E10:E51">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N45">
+  <conditionalFormatting sqref="N2:N46">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"y"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added LCSC and JLC purchases to BOM
</commit_message>
<xml_diff>
--- a/Hardware/Cornverter LCSC BOM.xlsx
+++ b/Hardware/Cornverter LCSC BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Cornverter\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A59309B-DF30-4920-9591-E1305E9A68D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97376C9-043A-4891-902D-802D3AACEE4F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{33667046-9C3D-47AC-83F4-8537F7000775}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="126">
   <si>
     <t>Quantity</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t>C100114</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -836,11 +839,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F513871-9508-4665-AE19-3C0D704DA94E}">
-  <dimension ref="A1:N56"/>
+  <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomLeft" activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,6 +1154,9 @@
         <f>(A2*M2)+(A4*M4)+(A6*M6)+(A8*M8)</f>
         <v>39</v>
       </c>
+      <c r="N10" s="1" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1196,6 +1202,9 @@
         <f>(A3*M3)+(A5*M5)+(A7*M7)+(A9*M9)</f>
         <v>37</v>
       </c>
+      <c r="N11" s="1" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -1235,6 +1244,9 @@
       <c r="K12" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="N12" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -1272,6 +1284,9 @@
       </c>
       <c r="K13" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1311,6 +1326,9 @@
       <c r="K14" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="N14" s="1" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -1345,6 +1363,9 @@
       </c>
       <c r="J15" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1387,6 +1408,9 @@
       <c r="L16" s="7">
         <v>0.05</v>
       </c>
+      <c r="N16" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -1428,6 +1452,9 @@
       <c r="L17" s="7">
         <v>0.05</v>
       </c>
+      <c r="N17" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -1469,6 +1496,9 @@
       <c r="L18" s="7">
         <v>0.05</v>
       </c>
+      <c r="N18" s="1" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -1510,6 +1540,9 @@
       <c r="L19" s="7">
         <v>0.05</v>
       </c>
+      <c r="N19" s="1" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -1548,6 +1581,9 @@
       <c r="K20" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="N20" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -1586,6 +1622,9 @@
       <c r="K21" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="N21" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
@@ -1624,7 +1663,7 @@
       <c r="K22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N22" s="2" t="s">
+      <c r="N22" s="1" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1664,6 +1703,9 @@
       </c>
       <c r="K23" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1703,6 +1745,9 @@
       <c r="K24" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="N24" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -1744,6 +1789,9 @@
       <c r="L25" s="7" t="s">
         <v>84</v>
       </c>
+      <c r="N25" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -1781,6 +1829,9 @@
       </c>
       <c r="K26" s="2" t="s">
         <v>86</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -1820,6 +1871,9 @@
       <c r="K27" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="N27" s="1" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
@@ -1858,6 +1912,9 @@
       <c r="K28" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="N28" s="1" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -1899,6 +1956,9 @@
       <c r="L29" s="7">
         <v>0.01</v>
       </c>
+      <c r="N29" s="1" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -1939,6 +1999,9 @@
       </c>
       <c r="L30" s="7">
         <v>0.01</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -1981,6 +2044,9 @@
       <c r="L31" s="7">
         <v>0.01</v>
       </c>
+      <c r="N31" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
@@ -2022,8 +2088,11 @@
       <c r="L32" s="7">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N32" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>2</v>
       </c>
@@ -2063,8 +2132,11 @@
       <c r="L33" s="7">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N33" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>1</v>
       </c>
@@ -2104,8 +2176,11 @@
       <c r="L34" s="7">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N34" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>22</v>
       </c>
@@ -2145,8 +2220,11 @@
       <c r="L35" s="7">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N35" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>3</v>
       </c>
@@ -2186,8 +2264,11 @@
       <c r="L36" s="7">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N36" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>8</v>
       </c>
@@ -2227,8 +2308,11 @@
       <c r="L37" s="7">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N37" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>2</v>
       </c>
@@ -2265,8 +2349,11 @@
       <c r="K38" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N38" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>4</v>
       </c>
@@ -2303,8 +2390,11 @@
       <c r="K39" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N39" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>2</v>
       </c>
@@ -2341,8 +2431,11 @@
       <c r="K40" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N40" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>1</v>
       </c>
@@ -2379,8 +2472,11 @@
       <c r="K41" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N41" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>1</v>
       </c>
@@ -2417,8 +2513,11 @@
       <c r="K42" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N42" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>18</v>
       </c>
@@ -2457,7 +2556,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>1</v>
       </c>
@@ -2496,7 +2595,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <f>D43+D44</f>
         <v>45</v>
@@ -2526,7 +2625,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <f>B45</f>
         <v>45</v>
@@ -2556,7 +2655,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E47" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2566,7 +2665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>1</v>
       </c>
@@ -2713,6 +2812,31 @@
       </c>
       <c r="B56" s="8">
         <v>3.72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57" s="8">
+        <v>7.49</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="8">
+        <v>12.18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="8">
+        <f>SUM(B56:B58)</f>
+        <v>23.39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Thonk order to BOM file
</commit_message>
<xml_diff>
--- a/Hardware/Cornverter LCSC BOM.xlsx
+++ b/Hardware/Cornverter LCSC BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Cornverter\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97376C9-043A-4891-902D-802D3AACEE4F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D8E40C-45FD-4B8B-B08F-619D30B83265}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{33667046-9C3D-47AC-83F4-8537F7000775}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="126">
   <si>
     <t>Quantity</t>
   </si>
@@ -418,7 +418,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,8 +450,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -464,6 +471,11 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -474,12 +486,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -505,9 +518,13 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{CA88BD54-F734-41BA-967D-5A9BFDB6E4F4}"/>
   </cellStyles>
@@ -839,11 +856,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F513871-9508-4665-AE19-3C0D704DA94E}">
-  <dimension ref="A1:N60"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O44" sqref="O44"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2555,6 +2572,9 @@
       <c r="K43" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="N43" s="9" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
@@ -2593,6 +2613,9 @@
       </c>
       <c r="K44" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="N44" s="9" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -2624,6 +2647,9 @@
       <c r="J45" s="2" t="s">
         <v>107</v>
       </c>
+      <c r="N45" s="9" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
@@ -2654,6 +2680,9 @@
       <c r="J46" s="2" t="s">
         <v>108</v>
       </c>
+      <c r="N46" s="9" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E47" s="2" t="str">
@@ -2830,13 +2859,21 @@
         <v>12.18</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" s="8">
+        <v>22.74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B60" s="8">
-        <f>SUM(B56:B58)</f>
-        <v>23.39</v>
+      <c r="B61" s="8">
+        <f>SUM(B56:B59)</f>
+        <v>46.129999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>